<commit_message>
preprocessing and feature select modified
</commit_message>
<xml_diff>
--- a/feature_select/feature_tests.xlsx
+++ b/feature_select/feature_tests.xlsx
@@ -469,508 +469,608 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sex</t>
+          <t>Number of Cigarettes Beedi per day</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11.53454624583081</v>
+        <v>-5.590892283513144</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0006831474935969359</v>
+        <v>5.98009298650165e-08</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Number of years smoked</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7.458947297404109e-07</v>
+        <v>-3.733747506234556</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9993109055108372</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
+        <v>0.0002302766207072653</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Admission Time</t>
+          <t>Height</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5220809801768388</v>
+        <v>1.744891299187858</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6020760192082126</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
+        <v>0.08218919358353449</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>father</t>
+          <t>Weight</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.4240332651805472</v>
+        <v>2.913267965563889</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5149313535052109</v>
-      </c>
-      <c r="D6" t="inlineStr"/>
+        <v>0.003869249071152921</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>mother</t>
+          <t>Heart_Rate</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.437007575527429</v>
+        <v>-3.234362666501038</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1185020950231579</v>
-      </c>
-      <c r="D7" t="inlineStr"/>
+        <v>0.001383804588752184</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>firstdeg</t>
+          <t>BP_Systolic</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0005331247262204686</v>
+        <v>6.042188989871409</v>
       </c>
       <c r="C8" t="n">
-        <v>0.98157888614725</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
+        <v>5.73848486163851e-09</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>seconddeg</t>
+          <t>BP_Diastolic</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.02521408139364543</v>
+        <v>5.59028242181165</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8738347809710847</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
+        <v>6.244306992381806e-08</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Atrial fib flutter</t>
+          <t>Exact Time of Symptom Onset</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>-0.3236946377134959</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
+        <v>0.7464310073287435</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Heart Failure</t>
+          <t>BASELINE SERUM CREATININE</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.313333360732582</v>
+        <v>-0.7613222658070451</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2517920180003121</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
+        <v>0.4472145015489534</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PriorPCI</t>
+          <t>HAEMOGLOBIN</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.0101333168749623</v>
+        <v>1.243247382274485</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9198168904122365</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
+        <v>0.2149193863498248</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Diabetes Mellitus</t>
+          <t>HBA1C</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>37.88543291702035</v>
+        <v>4.759889789535324</v>
       </c>
       <c r="C13" t="n">
-        <v>7.502333406120172e-10</v>
+        <v>3.124698435258619e-06</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Cancer</t>
+          <t>Total_cholesterol</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.313333360732582</v>
+        <v>0.3677038928963029</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2517920180003121</v>
-      </c>
-      <c r="D14" t="inlineStr"/>
+        <v>0.7134078712283751</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Hypertension</t>
+          <t>LDL</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>14.9982716274579</v>
+        <v>0.7105450493602388</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0001076096896880798</v>
+        <v>0.4780315764987272</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Prior CABG</t>
+          <t>HDL</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>0.03396153116542273</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" t="inlineStr"/>
+        <v>0.9729337806180898</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Hyperlipidemia</t>
+          <t>Triglycerides</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1.539397352293505</v>
+        <v>0.3050549226893559</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2147075303514012</v>
-      </c>
-      <c r="D17" t="inlineStr"/>
+        <v>0.7605726939516165</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PAD</t>
+          <t>APO B(g/l)</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.2972863886063807</v>
+        <v>5.243420237720859</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5855886337445986</v>
-      </c>
-      <c r="D18" t="inlineStr"/>
+        <v>3.180989585011831e-07</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Prior CVA</t>
+          <t>Liporotein A</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>3.446608394388543</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" t="inlineStr"/>
+        <v>0.000656396260328045</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Prior Angina</t>
+          <t>Admission Time</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.970802897550447</v>
+        <v>0.5220809801768388</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1603626647084065</v>
-      </c>
-      <c r="D20" t="inlineStr"/>
+        <v>0.6020760192082126</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Physical_Activity</t>
+          <t>Sex</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>8.698961368758162</v>
+        <v>11.53454624583081</v>
       </c>
       <c r="C21" t="n">
-        <v>0.003183914166166145</v>
+        <v>0.0006831474935969359</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Average_Sleep_Duration</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>5.541275981347471</v>
+        <v>7.458947297404109e-07</v>
       </c>
       <c r="C22" t="n">
-        <v>0.06262203971754214</v>
-      </c>
-      <c r="D22" t="inlineStr"/>
+        <v>0.9993109055108372</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Stress_Home</t>
+          <t>father</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>3.65798557223285</v>
+        <v>0.4240332651805472</v>
       </c>
       <c r="C23" t="n">
-        <v>0.3008425266173504</v>
-      </c>
-      <c r="D23" t="inlineStr"/>
+        <v>0.5149313535052109</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Stress_Work_Related</t>
+          <t>mother</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>8.668355206434674</v>
+        <v>2.437007575527429</v>
       </c>
       <c r="C24" t="n">
-        <v>0.03404125704829553</v>
-      </c>
-      <c r="D24" t="inlineStr"/>
+        <v>0.1185020950231579</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Stress_General</t>
+          <t>firstdeg</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>4.788872742492066</v>
+        <v>0.0005331247262204686</v>
       </c>
       <c r="C25" t="n">
-        <v>0.1879259858493902</v>
-      </c>
-      <c r="D25" t="inlineStr"/>
+        <v>0.98157888614725</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Tobacco_Use</t>
+          <t>seconddeg</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>47.98478674580767</v>
+        <v>0.02521408139364543</v>
       </c>
       <c r="C26" t="n">
-        <v>2.14541417487013e-10</v>
+        <v>0.8738347809710847</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Beedi</t>
+          <t>Atrial fib flutter</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>32.6689849648201</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>1.092669143339376e-08</v>
+        <v>1</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Cigarette</t>
+          <t>Heart Failure</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>5.059024283306032</v>
+        <v>1.313333360732582</v>
       </c>
       <c r="C28" t="n">
-        <v>0.02449802660579986</v>
-      </c>
-      <c r="D28" t="inlineStr"/>
+        <v>0.2517920180003121</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Hookah</t>
+          <t>PriorPCI</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
+        <v>0.0101333168749623</v>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" t="inlineStr"/>
+        <v>0.9198168904122365</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Tobacco Chewing</t>
+          <t>Diabetes Mellitus</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.4368060456658731</v>
+        <v>37.88543291702035</v>
       </c>
       <c r="C30" t="n">
-        <v>0.5086680833308559</v>
-      </c>
-      <c r="D30" t="inlineStr"/>
+        <v>7.502333406120172e-10</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Multiple </t>
+          <t>Cancer</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2.831938922127909</v>
+        <v>1.313333360732582</v>
       </c>
       <c r="C31" t="n">
-        <v>0.09240673341195649</v>
-      </c>
-      <c r="D31" t="inlineStr"/>
+        <v>0.2517920180003121</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Number of Cigarettes Beedi per day</t>
+          <t>Hypertension</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-5.590892283513144</v>
+        <v>14.9982716274579</v>
       </c>
       <c r="C32" t="n">
-        <v>5.98009298650165e-08</v>
+        <v>0.0001076096896880798</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Number of years smoked</t>
+          <t>Prior CABG</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-3.733747506234556</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>0.0002302766207072653</v>
+        <v>1</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Alcohol</t>
+          <t>Hyperlipidemia</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>4.100253169337439</v>
+        <v>1.539397352293505</v>
       </c>
       <c r="C34" t="n">
-        <v>0.2508401093429057</v>
-      </c>
-      <c r="D34" t="inlineStr"/>
+        <v>0.2147075303514012</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Gym_Supplements</t>
+          <t>PAD</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.5381922819352501</v>
+        <v>0.2972863886063807</v>
       </c>
       <c r="C35" t="n">
-        <v>0.4631828704418429</v>
-      </c>
-      <c r="D35" t="inlineStr"/>
+        <v>0.5855886337445986</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Cannabis</t>
+          <t>Prior CVA</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -979,879 +1079,1019 @@
       <c r="C36" t="n">
         <v>1</v>
       </c>
-      <c r="D36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Walking</t>
+          <t>Prior Angina</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.3329049314527511</v>
+        <v>1.970802897550447</v>
       </c>
       <c r="C37" t="n">
-        <v>0.8466630614925669</v>
-      </c>
-      <c r="D37" t="inlineStr"/>
+        <v>0.1603626647084065</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ASPRIN</t>
+          <t>Physical_Activity</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>8.749033671628233</v>
+        <v>8.698961368758162</v>
       </c>
       <c r="C38" t="n">
-        <v>0.00309766155277315</v>
+        <v>0.003183914166166145</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>STATIN</t>
+          <t>Average_Sleep_Duration</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>6.191520826578211</v>
+        <v>5.541275981347471</v>
       </c>
       <c r="C39" t="n">
-        <v>0.0128363826795191</v>
-      </c>
-      <c r="D39" t="inlineStr"/>
+        <v>0.06262203971754214</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>P2Y12 Inhibitors</t>
+          <t>Stress_Home</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
+        <v>3.65798557223285</v>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
-      </c>
-      <c r="D40" t="inlineStr"/>
+        <v>0.3008425266173504</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Beta_blocker</t>
+          <t>Stress_Work_Related</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.6275470576711925</v>
+        <v>8.668355206434674</v>
       </c>
       <c r="C41" t="n">
-        <v>0.4282564993284859</v>
-      </c>
-      <c r="D41" t="inlineStr"/>
+        <v>0.03404125704829553</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CalciumChannel</t>
+          <t>Stress_General</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.6801213337250624</v>
+        <v>4.788872742492066</v>
       </c>
       <c r="C42" t="n">
-        <v>0.4095449464260514</v>
-      </c>
-      <c r="D42" t="inlineStr"/>
+        <v>0.1879259858493902</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ACE ARB</t>
+          <t>Tobacco_Use</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.9024072561746328</v>
+        <v>47.98478674580767</v>
       </c>
       <c r="C43" t="n">
-        <v>0.3421370563648333</v>
-      </c>
-      <c r="D43" t="inlineStr"/>
+        <v>2.14541417487013e-10</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Aldosterone Blocking Antagonist</t>
+          <t>Beedi</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.2750203661656409</v>
+        <v>32.6689849648201</v>
       </c>
       <c r="C44" t="n">
-        <v>0.59998377718288</v>
-      </c>
-      <c r="D44" t="inlineStr"/>
+        <v>1.092669143339376e-08</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Anticoagulant</t>
+          <t>Cigarette</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.05225432383535633</v>
+        <v>5.059024283306032</v>
       </c>
       <c r="C45" t="n">
-        <v>0.8191860066901225</v>
-      </c>
-      <c r="D45" t="inlineStr"/>
+        <v>0.02449802660579986</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>INSULIN</t>
+          <t>Hookah</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>1.519484942763439</v>
+        <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>0.2176974533989677</v>
-      </c>
-      <c r="D46" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Oral Anti glycemics</t>
+          <t>Tobacco Chewing</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1.977110555838218</v>
+        <v>0.4368060456658731</v>
       </c>
       <c r="C47" t="n">
-        <v>0.9217916497222836</v>
-      </c>
-      <c r="D47" t="inlineStr"/>
+        <v>0.5086680833308559</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Homeopathy</t>
+          <t xml:space="preserve">Multiple </t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.02521408139364543</v>
+        <v>2.831938922127909</v>
       </c>
       <c r="C48" t="n">
-        <v>0.8738347809710847</v>
-      </c>
-      <c r="D48" t="inlineStr"/>
+        <v>0.09240673341195649</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Ayurveda</t>
+          <t>Alcohol</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.3063863390166748</v>
+        <v>4.100253169337439</v>
       </c>
       <c r="C49" t="n">
-        <v>0.5799061844172272</v>
-      </c>
-      <c r="D49" t="inlineStr"/>
+        <v>0.2508401093429057</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Symptoms_name</t>
+          <t>Gym_Supplements</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>5.660246757612585</v>
+        <v>0.5381922819352501</v>
       </c>
       <c r="C50" t="n">
-        <v>0.2259986253286266</v>
-      </c>
-      <c r="D50" t="inlineStr"/>
+        <v>0.4631828704418429</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>PRECEDING_ACTIVITY</t>
+          <t>Cannabis</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>4.120460277866981</v>
+        <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>0.1274246411490926</v>
-      </c>
-      <c r="D51" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>CardiacStatus_Presentation</t>
+          <t>Walking</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>131.842149346013</v>
+        <v>0.3329049314527511</v>
       </c>
       <c r="C52" t="n">
-        <v>2.348772905298489e-29</v>
+        <v>0.8466630614925669</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Exact Time of Symptom Onset</t>
+          <t>ASPRIN</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>-0.3236946377134959</v>
+        <v>8.749033671628233</v>
       </c>
       <c r="C53" t="n">
-        <v>0.7464310073287435</v>
-      </c>
-      <c r="D53" t="inlineStr"/>
+        <v>0.00309766155277315</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Time since symptoms onset to first medical contact</t>
+          <t>STATIN</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>5.583627178349474</v>
+        <v>6.191520826578211</v>
       </c>
       <c r="C54" t="n">
-        <v>0.2324757954505293</v>
-      </c>
-      <c r="D54" t="inlineStr"/>
+        <v>0.0128363826795191</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Mode_of_transport</t>
+          <t>P2Y12 Inhibitors</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>6.837449679819033</v>
+        <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>0.03275417513757838</v>
-      </c>
-      <c r="D55" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Type of First Medical Contact</t>
+          <t>Beta_blocker</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.08839823529958726</v>
+        <v>0.6275470576711925</v>
       </c>
       <c r="C56" t="n">
-        <v>0.7662234297399017</v>
-      </c>
-      <c r="D56" t="inlineStr"/>
+        <v>0.4282564993284859</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Nature of Treatment</t>
+          <t>CalciumChannel</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>2.949544823387907</v>
+        <v>0.6801213337250624</v>
       </c>
       <c r="C57" t="n">
-        <v>0.2288308003335811</v>
-      </c>
-      <c r="D57" t="inlineStr"/>
+        <v>0.4095449464260514</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Height</t>
+          <t>ACE ARB</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>1.744891299187858</v>
+        <v>0.9024072561746328</v>
       </c>
       <c r="C58" t="n">
-        <v>0.08218919358353449</v>
-      </c>
-      <c r="D58" t="inlineStr"/>
+        <v>0.3421370563648333</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Weight</t>
+          <t>Aldosterone Blocking Antagonist</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>2.913267965563889</v>
+        <v>0.2750203661656409</v>
       </c>
       <c r="C59" t="n">
-        <v>0.003869249071152921</v>
+        <v>0.59998377718288</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Heart_Rate</t>
+          <t>Anticoagulant</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-3.234362666501038</v>
+        <v>0.05225432383535633</v>
       </c>
       <c r="C60" t="n">
-        <v>0.001383804588752184</v>
+        <v>0.8191860066901225</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>BP_Systolic</t>
+          <t>INSULIN</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>6.042188989871409</v>
+        <v>1.519484942763439</v>
       </c>
       <c r="C61" t="n">
-        <v>5.73848486163851e-09</v>
+        <v>0.2176974533989677</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>BP_Diastolic</t>
+          <t>Oral Anti glycemics</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>5.59028242181165</v>
+        <v>1.977110555838218</v>
       </c>
       <c r="C62" t="n">
-        <v>6.244306992381806e-08</v>
+        <v>0.9217916497222836</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Time_since_symptom_onset_to_1st_ECG</t>
+          <t>Homeopathy</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>28.100467478619</v>
+        <v>0.02521408139364543</v>
       </c>
       <c r="C63" t="n">
-        <v>0.1070423468484593</v>
-      </c>
-      <c r="D63" t="inlineStr"/>
+        <v>0.8738347809710847</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>MItype_on_ECG</t>
+          <t>Ayurveda</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.343546349347515</v>
+        <v>0.3063863390166748</v>
       </c>
       <c r="C64" t="n">
-        <v>0.9516408965497388</v>
-      </c>
-      <c r="D64" t="inlineStr"/>
+        <v>0.5799061844172272</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Beta blocker</t>
+          <t>Symptoms_name</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>14.09700642208352</v>
+        <v>5.660246757612585</v>
       </c>
       <c r="C65" t="n">
-        <v>0.006991801200777611</v>
+        <v>0.2259986253286266</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>THROMBOLYSIS</t>
+          <t>PRECEDING_ACTIVITY</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.3712141776394673</v>
+        <v>4.120460277866981</v>
       </c>
       <c r="C66" t="n">
-        <v>0.5423431800732004</v>
-      </c>
-      <c r="D66" t="inlineStr"/>
+        <v>0.1274246411490926</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>RWMA</t>
+          <t>CardiacStatus_Presentation</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.003580054935816004</v>
+        <v>131.842149346013</v>
       </c>
       <c r="C67" t="n">
-        <v>0.9522881962113109</v>
-      </c>
-      <c r="D67" t="inlineStr"/>
+        <v>2.348772905298489e-29</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>EJECTION FRACTION(%)</t>
+          <t>Time since symptoms onset to first medical contact</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>43.9521120369062</v>
+        <v>5.583627178349474</v>
       </c>
       <c r="C68" t="n">
-        <v>2.368652670345275e-08</v>
+        <v>0.2324757954505293</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>PRESENCE OF MITRAL REGURGITATION</t>
+          <t>Mode_of_transport</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>287.893173379495</v>
+        <v>6.837449679819033</v>
       </c>
       <c r="C69" t="n">
-        <v>4.148090291191982e-62</v>
+        <v>0.03275417513757838</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>LV THROMBUS</t>
+          <t>Type of First Medical Contact</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>38.27184073954347</v>
+        <v>0.08839823529958726</v>
       </c>
       <c r="C70" t="n">
-        <v>6.154437157779015e-10</v>
+        <v>0.7662234297399017</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>VSD</t>
+          <t>Nature of Treatment</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>49.29718448025415</v>
+        <v>2.949544823387907</v>
       </c>
       <c r="C71" t="n">
-        <v>2.199779925357968e-12</v>
+        <v>0.2288308003335811</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>LV ANEURYSM</t>
+          <t>MItype_on_ECG</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>63.30150418350568</v>
+        <v>0.343546349347515</v>
       </c>
       <c r="C72" t="n">
-        <v>1.773688145390625e-15</v>
+        <v>0.9516408965497388</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>ACUTE_MR</t>
+          <t>Beta blocker</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>72.80180783603235</v>
+        <v>14.09700642208352</v>
       </c>
       <c r="C73" t="n">
-        <v>1.433454856537554e-17</v>
+        <v>0.006991801200777611</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>BASELINE SERUM CREATININE</t>
+          <t>THROMBOLYSIS</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>-0.7613222658070451</v>
+        <v>0.3712141776394673</v>
       </c>
       <c r="C74" t="n">
-        <v>0.4472145015489534</v>
-      </c>
-      <c r="D74" t="inlineStr"/>
+        <v>0.5423431800732004</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>HAEMOGLOBIN</t>
+          <t>RWMA</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>1.243247382274485</v>
+        <v>0.003580054935816004</v>
       </c>
       <c r="C75" t="n">
-        <v>0.2149193863498248</v>
-      </c>
-      <c r="D75" t="inlineStr"/>
+        <v>0.9522881962113109</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>HBA1C</t>
+          <t>Trop_T</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>4.759889789535324</v>
+        <v>0.03869922904611143</v>
       </c>
       <c r="C76" t="n">
-        <v>3.124698435258619e-06</v>
+        <v>0.8440457220124487</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Total_cholesterol</t>
+          <t>Coronary_angiography</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.3677038928963029</v>
+        <v>22.11050365478213</v>
       </c>
       <c r="C77" t="n">
-        <v>0.7134078712283751</v>
-      </c>
-      <c r="D77" t="inlineStr"/>
+        <v>1.580393137956131e-05</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>LDL</t>
+          <t>Age 65-74/&gt;75</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.7105450493602388</v>
+        <v>10.30475957431556</v>
       </c>
       <c r="C78" t="n">
-        <v>0.4780315764987272</v>
-      </c>
-      <c r="D78" t="inlineStr"/>
+        <v>0.00578561978706754</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>HDL</t>
+          <t>Systolic BP&lt;100</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.03396153116542273</v>
+        <v>73.06738965449915</v>
       </c>
       <c r="C79" t="n">
-        <v>0.9729337806180898</v>
-      </c>
-      <c r="D79" t="inlineStr"/>
+        <v>1.252977513975094e-17</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Triglycerides</t>
+          <t>Heart Rate&gt;100</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.3050549226893559</v>
+        <v>9.22928552801441</v>
       </c>
       <c r="C80" t="n">
-        <v>0.7605726939516165</v>
-      </c>
-      <c r="D80" t="inlineStr"/>
+        <v>0.002381745678264956</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>APO B(g/l)</t>
+          <t>KILLIP II-IV</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>5.243420237720859</v>
+        <v>63.73280259104504</v>
       </c>
       <c r="C81" t="n">
-        <v>3.180989585011831e-07</v>
+        <v>1.424920570267967e-15</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Liporotein A</t>
+          <t>Anterior STE or LBBB</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>3.446608394388543</v>
+        <v>0.03188344315498007</v>
       </c>
       <c r="C82" t="n">
-        <v>0.000656396260328045</v>
+        <v>0.8582837117260116</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Trop_T</t>
+          <t>H/O Diabetes, HTN or Angina</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.03869922904611143</v>
+        <v>42.36740648436264</v>
       </c>
       <c r="C83" t="n">
-        <v>0.8440457220124487</v>
-      </c>
-      <c r="D83" t="inlineStr"/>
+        <v>7.564013375814875e-11</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Coronary_angiography</t>
+          <t>Weight &lt; 67 Kgs</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>22.11050365478213</v>
+        <v>4.808093441574595</v>
       </c>
       <c r="C84" t="n">
-        <v>1.580393137956131e-05</v>
+        <v>0.02832636798905187</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Age 65-74/&gt;75</t>
+          <t>Time to Treatment &gt;4 Hours</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>10.30475957431556</v>
+        <v>5.145881977272849</v>
       </c>
       <c r="C85" t="n">
-        <v>0.00578561978706754</v>
+        <v>0.02330157078029437</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Systolic BP&lt;100</t>
+          <t>EJECTION FRACTION(%)</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>73.06738965449915</v>
+        <v>43.9521120369062</v>
       </c>
       <c r="C86" t="n">
-        <v>1.252977513975094e-17</v>
+        <v>2.368652670345275e-08</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Heart Rate&gt;100</t>
+          <t>PRESENCE OF MITRAL REGURGITATION</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>9.22928552801441</v>
+        <v>287.893173379495</v>
       </c>
       <c r="C87" t="n">
-        <v>0.002381745678264956</v>
+        <v>4.148090291191982e-62</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>KILLIP II-IV</t>
+          <t>LV THROMBUS</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>63.73280259104504</v>
+        <v>38.27184073954347</v>
       </c>
       <c r="C88" t="n">
-        <v>1.424920570267967e-15</v>
+        <v>6.154437157779015e-10</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Anterior STE or LBBB</t>
+          <t>VSD</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.03188344315498007</v>
+        <v>49.29718448025415</v>
       </c>
       <c r="C89" t="n">
-        <v>0.8582837117260116</v>
-      </c>
-      <c r="D89" t="inlineStr"/>
+        <v>2.199779925357968e-12</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>H/O Diabetes, HTN or Angina</t>
+          <t>LV ANEURYSM</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>42.36740648436264</v>
+        <v>63.30150418350568</v>
       </c>
       <c r="C90" t="n">
-        <v>7.564013375814875e-11</v>
+        <v>1.773688145390625e-15</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Significant</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Weight &lt; 67 Kgs</t>
+          <t>ACUTE_MR</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>4.808093441574595</v>
+        <v>72.80180783603235</v>
       </c>
       <c r="C91" t="n">
-        <v>0.02832636798905187</v>
-      </c>
-      <c r="D91" t="inlineStr"/>
+        <v>1.433454856537554e-17</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Time to Treatment &gt;4 Hours</t>
+          <t>Time_since_symptom_onset_to_1st_ECG</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>5.145881977272849</v>
+        <v>28.100467478619</v>
       </c>
       <c r="C92" t="n">
-        <v>0.02330157078029437</v>
-      </c>
-      <c r="D92" t="inlineStr"/>
+        <v>0.1070423468484593</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>